<commit_message>
feat: Update dataset and standards
</commit_message>
<xml_diff>
--- a/data/Yuanjing_Data_Standard_Ultimate_Final.xlsx
+++ b/data/Yuanjing_Data_Standard_Ultimate_Final.xlsx
@@ -1,26 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project Demo\Original-Mirror\MultiChannel-Reasoning-System\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8672BA7A-5802-4509-B5FD-BFD985E6C78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{DE9C3A46-5205-4CEC-9911-58899266A521}"/>
+    <workbookView windowWidth="25600" windowHeight="11360"/>
   </bookViews>
   <sheets>
     <sheet name="Yuanjing_Data_Standard_Final (v" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="293">
   <si>
     <t>ID</t>
   </si>
@@ -904,38 +911,71 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="等线 Light"/>
-      <family val="2"/>
+      <name val="Calibri Light"/>
       <charset val="134"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="等线"/>
-      <family val="2"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -943,8 +983,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="等线"/>
-      <family val="2"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -952,40 +991,14 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="等线"/>
-      <family val="2"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <family val="2"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -993,8 +1006,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <family val="2"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1002,16 +1014,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <family val="2"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1019,25 +1022,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="等线"/>
-      <family val="2"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <family val="2"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1045,23 +1037,35 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="2"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1075,175 +1079,188 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1253,6 +1270,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1278,7 +1310,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.399975585192419"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1313,15 +1345,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1337,17 +1360,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1363,131 +1380,152 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1496,61 +1534,71 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="着色 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="着色 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="着色 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="着色 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="着色 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
+  <cellStyles count="49">
+    <cellStyle name="常規" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="貨幣" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="貨幣[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超鏈接" xfId="6" builtinId="8"/>
+    <cellStyle name="已訪問的超鏈接" xfId="7" builtinId="9"/>
+    <cellStyle name="註釋" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文字" xfId="9" builtinId="11"/>
+    <cellStyle name="標題" xfId="10" builtinId="15"/>
+    <cellStyle name="解釋性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="標題 1" xfId="12" builtinId="16"/>
+    <cellStyle name="標題 2" xfId="13" builtinId="17"/>
+    <cellStyle name="標題 3" xfId="14" builtinId="18"/>
+    <cellStyle name="標題 4" xfId="15" builtinId="19"/>
+    <cellStyle name="輸入" xfId="16" builtinId="20"/>
+    <cellStyle name="輸出" xfId="17" builtinId="21"/>
+    <cellStyle name="計算" xfId="18" builtinId="22"/>
+    <cellStyle name="檢查儲存格" xfId="19" builtinId="23"/>
+    <cellStyle name="鏈接儲存格" xfId="20" builtinId="24"/>
+    <cellStyle name="匯總" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="適中" xfId="24" builtinId="28"/>
+    <cellStyle name="強調文字顏色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 強調文字顏色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 強調文字顏色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 強調文字顏色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="強調文字顏色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 強調文字顏色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 強調文字顏色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 強調文字顏色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="強調文字顏色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 強調文字顏色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 強調文字顏色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 強調文字顏色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="強調文字顏色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 強調文字顏色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 強調文字顏色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 強調文字顏色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="強調文字顏色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 強調文字顏色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 強調文字顏色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 強調文字顏色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="強調文字顏色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 強調文字顏色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 強調文字顏色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 強調文字顏色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1596,7 +1644,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1629,26 +1677,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1681,23 +1712,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1839,44 +1853,39 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF33E5C-B485-4767-A42A-089A459944C6}">
-  <dimension ref="A1:P74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:P63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75:XFD84"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="105.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="76.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.55454545454545" customWidth="1"/>
+    <col min="2" max="2" width="13.3363636363636" customWidth="1"/>
+    <col min="3" max="3" width="34.2181818181818" customWidth="1"/>
+    <col min="4" max="4" width="105.554545454545" customWidth="1"/>
+    <col min="5" max="5" width="14.2181818181818" customWidth="1"/>
+    <col min="6" max="6" width="15.6636363636364" customWidth="1"/>
+    <col min="7" max="7" width="17.7818181818182" customWidth="1"/>
+    <col min="8" max="8" width="13.5545454545455" customWidth="1"/>
+    <col min="9" max="9" width="16.1090909090909" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="11" width="14.3363636363636" customWidth="1"/>
+    <col min="12" max="12" width="15.3363636363636" customWidth="1"/>
+    <col min="13" max="13" width="16.6636363636364" customWidth="1"/>
+    <col min="14" max="14" width="14.4454545454545" customWidth="1"/>
+    <col min="15" max="15" width="18.1090909090909" customWidth="1"/>
+    <col min="16" max="16" width="76.2181818181818" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1926,7 +1935,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1955,7 +1964,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1987,7 +1996,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2019,7 +2028,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2048,7 +2057,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2077,7 +2086,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2106,7 +2115,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2135,7 +2144,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2164,7 +2173,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2193,7 +2202,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2222,7 +2231,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2251,7 +2260,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2280,7 +2289,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2309,382 +2318,817 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="F15">
-        <v>1</v>
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>61</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="F16">
-        <v>1</v>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" t="s">
+        <v>64</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="F17">
-        <v>1</v>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" t="s">
+        <v>67</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="F18">
-        <v>1</v>
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" t="s">
+        <v>70</v>
       </c>
       <c r="G18">
         <v>1</v>
       </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="F19">
-        <v>1</v>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" t="s">
+        <v>73</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="P20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="D26" t="s">
-        <v>61</v>
-      </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
-      <c r="P26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-      <c r="P27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="D28" t="s">
-        <v>67</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-      <c r="P28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="C29" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="D29" t="s">
-        <v>70</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="P29" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
-      </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-      <c r="P30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="D31" t="s">
-        <v>76</v>
+        <v>101</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31" t="s">
+        <v>102</v>
+      </c>
+      <c r="J31" t="s">
+        <v>103</v>
+      </c>
+      <c r="K31" t="s">
+        <v>104</v>
+      </c>
+      <c r="L31" t="s">
+        <v>105</v>
+      </c>
+      <c r="M31" t="s">
+        <v>106</v>
+      </c>
+      <c r="N31" t="s">
+        <v>107</v>
+      </c>
+      <c r="O31" t="s">
+        <v>108</v>
       </c>
       <c r="P31" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="D32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32" t="s">
+        <v>102</v>
+      </c>
+      <c r="J32" t="s">
+        <v>112</v>
+      </c>
+      <c r="K32" t="s">
+        <v>104</v>
+      </c>
+      <c r="L32" t="s">
+        <v>105</v>
+      </c>
+      <c r="M32" t="s">
+        <v>106</v>
+      </c>
+      <c r="N32" t="s">
+        <v>107</v>
+      </c>
+      <c r="O32" t="s">
+        <v>105</v>
+      </c>
+      <c r="P32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C33" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="D33" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33" t="s">
+        <v>102</v>
+      </c>
+      <c r="J33" t="s">
+        <v>103</v>
+      </c>
+      <c r="K33" t="s">
+        <v>104</v>
+      </c>
+      <c r="L33" t="s">
+        <v>116</v>
+      </c>
+      <c r="M33" t="s">
+        <v>106</v>
+      </c>
+      <c r="N33" t="s">
+        <v>117</v>
+      </c>
+      <c r="O33" t="s">
+        <v>118</v>
+      </c>
+      <c r="P33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C34" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="D34" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34" t="s">
+        <v>102</v>
+      </c>
+      <c r="J34" t="s">
+        <v>103</v>
+      </c>
+      <c r="K34" t="s">
+        <v>121</v>
+      </c>
+      <c r="L34" t="s">
+        <v>122</v>
+      </c>
+      <c r="M34" t="s">
+        <v>106</v>
+      </c>
+      <c r="N34" t="s">
+        <v>107</v>
+      </c>
+      <c r="O34" t="s">
+        <v>123</v>
+      </c>
+      <c r="P34" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C35" t="s">
-        <v>85</v>
+        <v>125</v>
       </c>
       <c r="D35" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35" t="s">
+        <v>102</v>
+      </c>
+      <c r="J35" t="s">
+        <v>103</v>
+      </c>
+      <c r="K35" t="s">
+        <v>121</v>
+      </c>
+      <c r="L35" t="s">
+        <v>105</v>
+      </c>
+      <c r="M35" t="s">
+        <v>127</v>
+      </c>
+      <c r="N35" t="s">
+        <v>107</v>
+      </c>
+      <c r="O35" t="s">
+        <v>128</v>
+      </c>
+      <c r="P35" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C36" t="s">
-        <v>87</v>
+        <v>130</v>
       </c>
       <c r="D36" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36" t="s">
+        <v>102</v>
+      </c>
+      <c r="J36" t="s">
+        <v>112</v>
+      </c>
+      <c r="K36" t="s">
+        <v>121</v>
+      </c>
+      <c r="L36" t="s">
+        <v>107</v>
+      </c>
+      <c r="M36" t="s">
+        <v>132</v>
+      </c>
+      <c r="N36" t="s">
+        <v>107</v>
+      </c>
+      <c r="O36" t="s">
+        <v>133</v>
+      </c>
+      <c r="P36" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C37" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37" t="s">
+        <v>102</v>
+      </c>
+      <c r="J37" t="s">
+        <v>112</v>
+      </c>
+      <c r="K37" t="s">
+        <v>137</v>
+      </c>
+      <c r="L37" t="s">
+        <v>105</v>
+      </c>
+      <c r="M37" t="s">
+        <v>106</v>
+      </c>
+      <c r="N37" t="s">
+        <v>107</v>
+      </c>
+      <c r="O37" t="s">
+        <v>138</v>
+      </c>
+      <c r="P37" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C38" t="s">
-        <v>91</v>
+        <v>140</v>
       </c>
       <c r="D38" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38" t="s">
+        <v>102</v>
+      </c>
+      <c r="J38" t="s">
+        <v>103</v>
+      </c>
+      <c r="K38" t="s">
+        <v>142</v>
+      </c>
+      <c r="L38" t="s">
+        <v>122</v>
+      </c>
+      <c r="M38" t="s">
+        <v>106</v>
+      </c>
+      <c r="N38" t="s">
+        <v>143</v>
+      </c>
+      <c r="O38" t="s">
+        <v>144</v>
+      </c>
+      <c r="P38" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C39" t="s">
-        <v>93</v>
+        <v>146</v>
       </c>
       <c r="D39" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39" t="s">
+        <v>102</v>
+      </c>
+      <c r="J39" t="s">
+        <v>103</v>
+      </c>
+      <c r="K39" t="s">
+        <v>148</v>
+      </c>
+      <c r="L39" t="s">
+        <v>149</v>
+      </c>
+      <c r="M39" t="s">
+        <v>106</v>
+      </c>
+      <c r="N39" t="s">
+        <v>117</v>
+      </c>
+      <c r="O39" t="s">
+        <v>149</v>
+      </c>
+      <c r="P39" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C40" t="s">
-        <v>95</v>
+        <v>151</v>
       </c>
       <c r="D40" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40" t="s">
+        <v>102</v>
+      </c>
+      <c r="J40" t="s">
+        <v>103</v>
+      </c>
+      <c r="K40" t="s">
+        <v>122</v>
+      </c>
+      <c r="L40" t="s">
+        <v>153</v>
+      </c>
+      <c r="M40" t="s">
+        <v>154</v>
+      </c>
+      <c r="N40" t="s">
+        <v>143</v>
+      </c>
+      <c r="O40" t="s">
+        <v>155</v>
+      </c>
+      <c r="P40" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C41" t="s">
-        <v>97</v>
+        <v>157</v>
       </c>
       <c r="D41" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41" t="s">
+        <v>102</v>
+      </c>
+      <c r="J41" t="s">
+        <v>103</v>
+      </c>
+      <c r="K41" t="s">
+        <v>142</v>
+      </c>
+      <c r="L41" t="s">
+        <v>159</v>
+      </c>
+      <c r="M41" t="s">
+        <v>154</v>
+      </c>
+      <c r="N41" t="s">
+        <v>117</v>
+      </c>
+      <c r="O41" t="s">
+        <v>160</v>
+      </c>
+      <c r="P41" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2692,10 +3136,10 @@
         <v>99</v>
       </c>
       <c r="C42" t="s">
-        <v>100</v>
+        <v>162</v>
       </c>
       <c r="D42" t="s">
-        <v>101</v>
+        <v>163</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -2716,25 +3160,25 @@
         <v>103</v>
       </c>
       <c r="K42" t="s">
-        <v>104</v>
+        <v>148</v>
       </c>
       <c r="L42" t="s">
-        <v>105</v>
+        <v>164</v>
       </c>
       <c r="M42" t="s">
-        <v>106</v>
+        <v>165</v>
       </c>
       <c r="N42" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="O42" t="s">
-        <v>108</v>
+        <v>166</v>
       </c>
       <c r="P42" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2742,10 +3186,10 @@
         <v>99</v>
       </c>
       <c r="C43" t="s">
-        <v>110</v>
+        <v>168</v>
       </c>
       <c r="D43" t="s">
-        <v>111</v>
+        <v>169</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -2763,28 +3207,28 @@
         <v>102</v>
       </c>
       <c r="J43" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="K43" t="s">
-        <v>104</v>
+        <v>142</v>
       </c>
       <c r="L43" t="s">
-        <v>105</v>
+        <v>170</v>
       </c>
       <c r="M43" t="s">
-        <v>106</v>
+        <v>154</v>
       </c>
       <c r="N43" t="s">
         <v>107</v>
       </c>
       <c r="O43" t="s">
-        <v>105</v>
+        <v>171</v>
       </c>
       <c r="P43" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2792,10 +3236,10 @@
         <v>99</v>
       </c>
       <c r="C44" t="s">
-        <v>114</v>
+        <v>173</v>
       </c>
       <c r="D44" t="s">
-        <v>115</v>
+        <v>174</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -2813,28 +3257,28 @@
         <v>102</v>
       </c>
       <c r="J44" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="K44" t="s">
-        <v>104</v>
+        <v>137</v>
       </c>
       <c r="L44" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="M44" t="s">
-        <v>106</v>
+        <v>154</v>
       </c>
       <c r="N44" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="O44" t="s">
         <v>118</v>
       </c>
       <c r="P44" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2842,10 +3286,10 @@
         <v>99</v>
       </c>
       <c r="C45" t="s">
-        <v>119</v>
+        <v>176</v>
       </c>
       <c r="D45" t="s">
-        <v>120</v>
+        <v>177</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -2866,25 +3310,25 @@
         <v>103</v>
       </c>
       <c r="K45" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="L45" t="s">
-        <v>122</v>
+        <v>178</v>
       </c>
       <c r="M45" t="s">
-        <v>106</v>
+        <v>179</v>
       </c>
       <c r="N45" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="O45" t="s">
-        <v>123</v>
+        <v>180</v>
       </c>
       <c r="P45" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2892,10 +3336,10 @@
         <v>99</v>
       </c>
       <c r="C46" t="s">
-        <v>125</v>
+        <v>182</v>
       </c>
       <c r="D46" t="s">
-        <v>126</v>
+        <v>183</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -2916,25 +3360,25 @@
         <v>103</v>
       </c>
       <c r="K46" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L46" t="s">
-        <v>105</v>
+        <v>184</v>
       </c>
       <c r="M46" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="N46" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="O46" t="s">
-        <v>128</v>
+        <v>185</v>
       </c>
       <c r="P46" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2942,10 +3386,10 @@
         <v>99</v>
       </c>
       <c r="C47" t="s">
-        <v>130</v>
+        <v>187</v>
       </c>
       <c r="D47" t="s">
-        <v>131</v>
+        <v>188</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -2963,28 +3407,28 @@
         <v>102</v>
       </c>
       <c r="J47" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="K47" t="s">
-        <v>121</v>
+        <v>189</v>
       </c>
       <c r="L47" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="M47" t="s">
-        <v>132</v>
+        <v>190</v>
       </c>
       <c r="N47" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="O47" t="s">
-        <v>133</v>
+        <v>191</v>
       </c>
       <c r="P47" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2992,10 +3436,10 @@
         <v>99</v>
       </c>
       <c r="C48" t="s">
-        <v>135</v>
+        <v>193</v>
       </c>
       <c r="D48" t="s">
-        <v>136</v>
+        <v>194</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -3013,28 +3457,28 @@
         <v>102</v>
       </c>
       <c r="J48" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="K48" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="L48" t="s">
-        <v>105</v>
+        <v>195</v>
       </c>
       <c r="M48" t="s">
-        <v>106</v>
+        <v>196</v>
       </c>
       <c r="N48" t="s">
-        <v>107</v>
+        <v>197</v>
       </c>
       <c r="O48" t="s">
-        <v>138</v>
+        <v>198</v>
       </c>
       <c r="P48" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3042,10 +3486,10 @@
         <v>99</v>
       </c>
       <c r="C49" t="s">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="D49" t="s">
-        <v>141</v>
+        <v>201</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -3069,22 +3513,22 @@
         <v>142</v>
       </c>
       <c r="L49" t="s">
-        <v>122</v>
+        <v>202</v>
       </c>
       <c r="M49" t="s">
-        <v>106</v>
+        <v>203</v>
       </c>
       <c r="N49" t="s">
-        <v>143</v>
+        <v>197</v>
       </c>
       <c r="O49" t="s">
-        <v>144</v>
+        <v>204</v>
       </c>
       <c r="P49" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3092,10 +3536,10 @@
         <v>99</v>
       </c>
       <c r="C50" t="s">
-        <v>146</v>
+        <v>206</v>
       </c>
       <c r="D50" t="s">
-        <v>147</v>
+        <v>207</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -3119,22 +3563,22 @@
         <v>148</v>
       </c>
       <c r="L50" t="s">
-        <v>149</v>
+        <v>208</v>
       </c>
       <c r="M50" t="s">
-        <v>106</v>
+        <v>209</v>
       </c>
       <c r="N50" t="s">
-        <v>117</v>
+        <v>210</v>
       </c>
       <c r="O50" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="P50" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3142,10 +3586,10 @@
         <v>99</v>
       </c>
       <c r="C51" t="s">
-        <v>151</v>
+        <v>213</v>
       </c>
       <c r="D51" t="s">
-        <v>152</v>
+        <v>214</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -3166,25 +3610,25 @@
         <v>103</v>
       </c>
       <c r="K51" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="L51" t="s">
-        <v>153</v>
+        <v>215</v>
       </c>
       <c r="M51" t="s">
-        <v>154</v>
+        <v>216</v>
       </c>
       <c r="N51" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="O51" t="s">
-        <v>155</v>
+        <v>217</v>
       </c>
       <c r="P51" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3192,10 +3636,10 @@
         <v>99</v>
       </c>
       <c r="C52" t="s">
-        <v>157</v>
+        <v>219</v>
       </c>
       <c r="D52" t="s">
-        <v>158</v>
+        <v>220</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -3216,25 +3660,25 @@
         <v>103</v>
       </c>
       <c r="K52" t="s">
-        <v>142</v>
+        <v>221</v>
       </c>
       <c r="L52" t="s">
-        <v>159</v>
+        <v>222</v>
       </c>
       <c r="M52" t="s">
-        <v>154</v>
+        <v>223</v>
       </c>
       <c r="N52" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="O52" t="s">
-        <v>160</v>
+        <v>224</v>
       </c>
       <c r="P52" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3242,10 +3686,10 @@
         <v>99</v>
       </c>
       <c r="C53" t="s">
-        <v>162</v>
+        <v>226</v>
       </c>
       <c r="D53" t="s">
-        <v>163</v>
+        <v>227</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -3266,25 +3710,25 @@
         <v>103</v>
       </c>
       <c r="K53" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="L53" t="s">
-        <v>164</v>
+        <v>228</v>
       </c>
       <c r="M53" t="s">
-        <v>165</v>
+        <v>229</v>
       </c>
       <c r="N53" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="O53" t="s">
-        <v>166</v>
+        <v>230</v>
       </c>
       <c r="P53" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3292,10 +3736,10 @@
         <v>99</v>
       </c>
       <c r="C54" t="s">
-        <v>168</v>
+        <v>232</v>
       </c>
       <c r="D54" t="s">
-        <v>169</v>
+        <v>233</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -3319,22 +3763,22 @@
         <v>142</v>
       </c>
       <c r="L54" t="s">
-        <v>170</v>
+        <v>234</v>
       </c>
       <c r="M54" t="s">
-        <v>154</v>
+        <v>235</v>
       </c>
       <c r="N54" t="s">
-        <v>107</v>
+        <v>197</v>
       </c>
       <c r="O54" t="s">
-        <v>171</v>
+        <v>236</v>
       </c>
       <c r="P54" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3342,10 +3786,10 @@
         <v>99</v>
       </c>
       <c r="C55" t="s">
-        <v>173</v>
+        <v>238</v>
       </c>
       <c r="D55" t="s">
-        <v>174</v>
+        <v>239</v>
       </c>
       <c r="E55">
         <v>1</v>
@@ -3363,28 +3807,28 @@
         <v>102</v>
       </c>
       <c r="J55" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="K55" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="L55" t="s">
-        <v>105</v>
+        <v>240</v>
       </c>
       <c r="M55" t="s">
-        <v>154</v>
+        <v>241</v>
       </c>
       <c r="N55" t="s">
-        <v>107</v>
+        <v>242</v>
       </c>
       <c r="O55" t="s">
-        <v>118</v>
+        <v>243</v>
       </c>
       <c r="P55" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3392,10 +3836,10 @@
         <v>99</v>
       </c>
       <c r="C56" t="s">
-        <v>176</v>
+        <v>245</v>
       </c>
       <c r="D56" t="s">
-        <v>177</v>
+        <v>246</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -3416,25 +3860,25 @@
         <v>103</v>
       </c>
       <c r="K56" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="L56" t="s">
-        <v>178</v>
+        <v>247</v>
       </c>
       <c r="M56" t="s">
-        <v>179</v>
+        <v>248</v>
       </c>
       <c r="N56" t="s">
-        <v>117</v>
+        <v>210</v>
       </c>
       <c r="O56" t="s">
-        <v>180</v>
+        <v>249</v>
       </c>
       <c r="P56" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3442,10 +3886,10 @@
         <v>99</v>
       </c>
       <c r="C57" t="s">
-        <v>182</v>
+        <v>251</v>
       </c>
       <c r="D57" t="s">
-        <v>183</v>
+        <v>252</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -3466,25 +3910,25 @@
         <v>103</v>
       </c>
       <c r="K57" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="L57" t="s">
-        <v>184</v>
+        <v>253</v>
       </c>
       <c r="M57" t="s">
-        <v>154</v>
+        <v>254</v>
       </c>
       <c r="N57" t="s">
-        <v>143</v>
+        <v>255</v>
       </c>
       <c r="O57" t="s">
-        <v>185</v>
+        <v>256</v>
       </c>
       <c r="P57" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3492,10 +3936,10 @@
         <v>99</v>
       </c>
       <c r="C58" t="s">
-        <v>187</v>
+        <v>258</v>
       </c>
       <c r="D58" t="s">
-        <v>188</v>
+        <v>259</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -3516,25 +3960,25 @@
         <v>103</v>
       </c>
       <c r="K58" t="s">
-        <v>189</v>
+        <v>148</v>
       </c>
       <c r="L58" t="s">
         <v>116</v>
       </c>
       <c r="M58" t="s">
-        <v>190</v>
+        <v>254</v>
       </c>
       <c r="N58" t="s">
-        <v>117</v>
+        <v>255</v>
       </c>
       <c r="O58" t="s">
-        <v>191</v>
+        <v>260</v>
       </c>
       <c r="P58" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3542,10 +3986,10 @@
         <v>99</v>
       </c>
       <c r="C59" t="s">
-        <v>193</v>
+        <v>262</v>
       </c>
       <c r="D59" t="s">
-        <v>194</v>
+        <v>263</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -3566,25 +4010,25 @@
         <v>103</v>
       </c>
       <c r="K59" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="L59" t="s">
-        <v>195</v>
+        <v>264</v>
       </c>
       <c r="M59" t="s">
-        <v>196</v>
+        <v>265</v>
       </c>
       <c r="N59" t="s">
-        <v>197</v>
+        <v>266</v>
       </c>
       <c r="O59" t="s">
-        <v>198</v>
+        <v>267</v>
       </c>
       <c r="P59" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3592,10 +4036,10 @@
         <v>99</v>
       </c>
       <c r="C60" t="s">
-        <v>200</v>
+        <v>269</v>
       </c>
       <c r="D60" t="s">
-        <v>201</v>
+        <v>270</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -3616,25 +4060,25 @@
         <v>103</v>
       </c>
       <c r="K60" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="L60" t="s">
-        <v>202</v>
+        <v>271</v>
       </c>
       <c r="M60" t="s">
-        <v>203</v>
+        <v>272</v>
       </c>
       <c r="N60" t="s">
-        <v>197</v>
+        <v>255</v>
       </c>
       <c r="O60" t="s">
-        <v>204</v>
+        <v>273</v>
       </c>
       <c r="P60" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3642,10 +4086,10 @@
         <v>99</v>
       </c>
       <c r="C61" t="s">
-        <v>206</v>
+        <v>275</v>
       </c>
       <c r="D61" t="s">
-        <v>207</v>
+        <v>276</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -3666,25 +4110,25 @@
         <v>103</v>
       </c>
       <c r="K61" t="s">
-        <v>148</v>
+        <v>104</v>
       </c>
       <c r="L61" t="s">
-        <v>208</v>
+        <v>149</v>
       </c>
       <c r="M61" t="s">
-        <v>209</v>
+        <v>277</v>
       </c>
       <c r="N61" t="s">
-        <v>210</v>
+        <v>117</v>
       </c>
       <c r="O61" t="s">
-        <v>211</v>
+        <v>278</v>
       </c>
       <c r="P61" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3692,10 +4136,10 @@
         <v>99</v>
       </c>
       <c r="C62" t="s">
-        <v>213</v>
+        <v>280</v>
       </c>
       <c r="D62" t="s">
-        <v>214</v>
+        <v>281</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -3719,22 +4163,22 @@
         <v>142</v>
       </c>
       <c r="L62" t="s">
-        <v>215</v>
+        <v>282</v>
       </c>
       <c r="M62" t="s">
-        <v>216</v>
+        <v>283</v>
       </c>
       <c r="N62" t="s">
-        <v>107</v>
+        <v>284</v>
       </c>
       <c r="O62" t="s">
-        <v>217</v>
+        <v>283</v>
       </c>
       <c r="P62" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3742,10 +4186,10 @@
         <v>99</v>
       </c>
       <c r="C63" t="s">
-        <v>219</v>
+        <v>286</v>
       </c>
       <c r="D63" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -3766,576 +4210,26 @@
         <v>103</v>
       </c>
       <c r="K63" t="s">
-        <v>221</v>
+        <v>142</v>
       </c>
       <c r="L63" t="s">
-        <v>222</v>
+        <v>288</v>
       </c>
       <c r="M63" t="s">
-        <v>223</v>
+        <v>289</v>
       </c>
       <c r="N63" t="s">
-        <v>107</v>
+        <v>290</v>
       </c>
       <c r="O63" t="s">
-        <v>224</v>
+        <v>291</v>
       </c>
       <c r="P63" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>63</v>
-      </c>
-      <c r="B64" t="s">
-        <v>99</v>
-      </c>
-      <c r="C64" t="s">
-        <v>226</v>
-      </c>
-      <c r="D64" t="s">
-        <v>227</v>
-      </c>
-      <c r="E64">
-        <v>1</v>
-      </c>
-      <c r="F64">
-        <v>0</v>
-      </c>
-      <c r="G64">
-        <v>0</v>
-      </c>
-      <c r="H64">
-        <v>1</v>
-      </c>
-      <c r="I64" t="s">
-        <v>102</v>
-      </c>
-      <c r="J64" t="s">
-        <v>103</v>
-      </c>
-      <c r="K64" t="s">
-        <v>142</v>
-      </c>
-      <c r="L64" t="s">
-        <v>228</v>
-      </c>
-      <c r="M64" t="s">
-        <v>229</v>
-      </c>
-      <c r="N64" t="s">
-        <v>105</v>
-      </c>
-      <c r="O64" t="s">
-        <v>230</v>
-      </c>
-      <c r="P64" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>64</v>
-      </c>
-      <c r="B65" t="s">
-        <v>99</v>
-      </c>
-      <c r="C65" t="s">
-        <v>232</v>
-      </c>
-      <c r="D65" t="s">
-        <v>233</v>
-      </c>
-      <c r="E65">
-        <v>1</v>
-      </c>
-      <c r="F65">
-        <v>0</v>
-      </c>
-      <c r="G65">
-        <v>0</v>
-      </c>
-      <c r="H65">
-        <v>1</v>
-      </c>
-      <c r="I65" t="s">
-        <v>102</v>
-      </c>
-      <c r="J65" t="s">
-        <v>103</v>
-      </c>
-      <c r="K65" t="s">
-        <v>142</v>
-      </c>
-      <c r="L65" t="s">
-        <v>234</v>
-      </c>
-      <c r="M65" t="s">
-        <v>235</v>
-      </c>
-      <c r="N65" t="s">
-        <v>197</v>
-      </c>
-      <c r="O65" t="s">
-        <v>236</v>
-      </c>
-      <c r="P65" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>65</v>
-      </c>
-      <c r="B66" t="s">
-        <v>99</v>
-      </c>
-      <c r="C66" t="s">
-        <v>238</v>
-      </c>
-      <c r="D66" t="s">
-        <v>239</v>
-      </c>
-      <c r="E66">
-        <v>1</v>
-      </c>
-      <c r="F66">
-        <v>0</v>
-      </c>
-      <c r="G66">
-        <v>0</v>
-      </c>
-      <c r="H66">
-        <v>1</v>
-      </c>
-      <c r="I66" t="s">
-        <v>102</v>
-      </c>
-      <c r="J66" t="s">
-        <v>103</v>
-      </c>
-      <c r="K66" t="s">
-        <v>142</v>
-      </c>
-      <c r="L66" t="s">
-        <v>240</v>
-      </c>
-      <c r="M66" t="s">
-        <v>241</v>
-      </c>
-      <c r="N66" t="s">
-        <v>242</v>
-      </c>
-      <c r="O66" t="s">
-        <v>243</v>
-      </c>
-      <c r="P66" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>66</v>
-      </c>
-      <c r="B67" t="s">
-        <v>99</v>
-      </c>
-      <c r="C67" t="s">
-        <v>245</v>
-      </c>
-      <c r="D67" t="s">
-        <v>246</v>
-      </c>
-      <c r="E67">
-        <v>1</v>
-      </c>
-      <c r="F67">
-        <v>0</v>
-      </c>
-      <c r="G67">
-        <v>0</v>
-      </c>
-      <c r="H67">
-        <v>1</v>
-      </c>
-      <c r="I67" t="s">
-        <v>102</v>
-      </c>
-      <c r="J67" t="s">
-        <v>103</v>
-      </c>
-      <c r="K67" t="s">
-        <v>142</v>
-      </c>
-      <c r="L67" t="s">
-        <v>247</v>
-      </c>
-      <c r="M67" t="s">
-        <v>248</v>
-      </c>
-      <c r="N67" t="s">
-        <v>210</v>
-      </c>
-      <c r="O67" t="s">
-        <v>249</v>
-      </c>
-      <c r="P67" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>67</v>
-      </c>
-      <c r="B68" t="s">
-        <v>99</v>
-      </c>
-      <c r="C68" t="s">
-        <v>251</v>
-      </c>
-      <c r="D68" t="s">
-        <v>252</v>
-      </c>
-      <c r="E68">
-        <v>1</v>
-      </c>
-      <c r="F68">
-        <v>0</v>
-      </c>
-      <c r="G68">
-        <v>0</v>
-      </c>
-      <c r="H68">
-        <v>1</v>
-      </c>
-      <c r="I68" t="s">
-        <v>102</v>
-      </c>
-      <c r="J68" t="s">
-        <v>103</v>
-      </c>
-      <c r="K68" t="s">
-        <v>142</v>
-      </c>
-      <c r="L68" t="s">
-        <v>253</v>
-      </c>
-      <c r="M68" t="s">
-        <v>254</v>
-      </c>
-      <c r="N68" t="s">
-        <v>255</v>
-      </c>
-      <c r="O68" t="s">
-        <v>256</v>
-      </c>
-      <c r="P68" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>68</v>
-      </c>
-      <c r="B69" t="s">
-        <v>99</v>
-      </c>
-      <c r="C69" t="s">
-        <v>258</v>
-      </c>
-      <c r="D69" t="s">
-        <v>259</v>
-      </c>
-      <c r="E69">
-        <v>1</v>
-      </c>
-      <c r="F69">
-        <v>0</v>
-      </c>
-      <c r="G69">
-        <v>0</v>
-      </c>
-      <c r="H69">
-        <v>1</v>
-      </c>
-      <c r="I69" t="s">
-        <v>102</v>
-      </c>
-      <c r="J69" t="s">
-        <v>103</v>
-      </c>
-      <c r="K69" t="s">
-        <v>148</v>
-      </c>
-      <c r="L69" t="s">
-        <v>116</v>
-      </c>
-      <c r="M69" t="s">
-        <v>254</v>
-      </c>
-      <c r="N69" t="s">
-        <v>255</v>
-      </c>
-      <c r="O69" t="s">
-        <v>260</v>
-      </c>
-      <c r="P69" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>69</v>
-      </c>
-      <c r="B70" t="s">
-        <v>99</v>
-      </c>
-      <c r="C70" t="s">
-        <v>262</v>
-      </c>
-      <c r="D70" t="s">
-        <v>263</v>
-      </c>
-      <c r="E70">
-        <v>1</v>
-      </c>
-      <c r="F70">
-        <v>0</v>
-      </c>
-      <c r="G70">
-        <v>0</v>
-      </c>
-      <c r="H70">
-        <v>1</v>
-      </c>
-      <c r="I70" t="s">
-        <v>102</v>
-      </c>
-      <c r="J70" t="s">
-        <v>103</v>
-      </c>
-      <c r="K70" t="s">
-        <v>122</v>
-      </c>
-      <c r="L70" t="s">
-        <v>264</v>
-      </c>
-      <c r="M70" t="s">
-        <v>265</v>
-      </c>
-      <c r="N70" t="s">
-        <v>266</v>
-      </c>
-      <c r="O70" t="s">
-        <v>267</v>
-      </c>
-      <c r="P70" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>70</v>
-      </c>
-      <c r="B71" t="s">
-        <v>99</v>
-      </c>
-      <c r="C71" t="s">
-        <v>269</v>
-      </c>
-      <c r="D71" t="s">
-        <v>270</v>
-      </c>
-      <c r="E71">
-        <v>1</v>
-      </c>
-      <c r="F71">
-        <v>0</v>
-      </c>
-      <c r="G71">
-        <v>0</v>
-      </c>
-      <c r="H71">
-        <v>1</v>
-      </c>
-      <c r="I71" t="s">
-        <v>102</v>
-      </c>
-      <c r="J71" t="s">
-        <v>103</v>
-      </c>
-      <c r="K71" t="s">
-        <v>148</v>
-      </c>
-      <c r="L71" t="s">
-        <v>271</v>
-      </c>
-      <c r="M71" t="s">
-        <v>272</v>
-      </c>
-      <c r="N71" t="s">
-        <v>255</v>
-      </c>
-      <c r="O71" t="s">
-        <v>273</v>
-      </c>
-      <c r="P71" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>71</v>
-      </c>
-      <c r="B72" t="s">
-        <v>99</v>
-      </c>
-      <c r="C72" t="s">
-        <v>275</v>
-      </c>
-      <c r="D72" t="s">
-        <v>276</v>
-      </c>
-      <c r="E72">
-        <v>1</v>
-      </c>
-      <c r="F72">
-        <v>0</v>
-      </c>
-      <c r="G72">
-        <v>0</v>
-      </c>
-      <c r="H72">
-        <v>1</v>
-      </c>
-      <c r="I72" t="s">
-        <v>102</v>
-      </c>
-      <c r="J72" t="s">
-        <v>103</v>
-      </c>
-      <c r="K72" t="s">
-        <v>104</v>
-      </c>
-      <c r="L72" t="s">
-        <v>149</v>
-      </c>
-      <c r="M72" t="s">
-        <v>277</v>
-      </c>
-      <c r="N72" t="s">
-        <v>117</v>
-      </c>
-      <c r="O72" t="s">
-        <v>278</v>
-      </c>
-      <c r="P72" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>72</v>
-      </c>
-      <c r="B73" t="s">
-        <v>99</v>
-      </c>
-      <c r="C73" t="s">
-        <v>280</v>
-      </c>
-      <c r="D73" t="s">
-        <v>281</v>
-      </c>
-      <c r="E73">
-        <v>1</v>
-      </c>
-      <c r="F73">
-        <v>0</v>
-      </c>
-      <c r="G73">
-        <v>0</v>
-      </c>
-      <c r="H73">
-        <v>1</v>
-      </c>
-      <c r="I73" t="s">
-        <v>102</v>
-      </c>
-      <c r="J73" t="s">
-        <v>103</v>
-      </c>
-      <c r="K73" t="s">
-        <v>142</v>
-      </c>
-      <c r="L73" t="s">
-        <v>282</v>
-      </c>
-      <c r="M73" t="s">
-        <v>283</v>
-      </c>
-      <c r="N73" t="s">
-        <v>284</v>
-      </c>
-      <c r="O73" t="s">
-        <v>283</v>
-      </c>
-      <c r="P73" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>73</v>
-      </c>
-      <c r="B74" t="s">
-        <v>99</v>
-      </c>
-      <c r="C74" t="s">
-        <v>286</v>
-      </c>
-      <c r="D74" t="s">
-        <v>287</v>
-      </c>
-      <c r="E74">
-        <v>1</v>
-      </c>
-      <c r="F74">
-        <v>0</v>
-      </c>
-      <c r="G74">
-        <v>0</v>
-      </c>
-      <c r="H74">
-        <v>1</v>
-      </c>
-      <c r="I74" t="s">
-        <v>102</v>
-      </c>
-      <c r="J74" t="s">
-        <v>103</v>
-      </c>
-      <c r="K74" t="s">
-        <v>142</v>
-      </c>
-      <c r="L74" t="s">
-        <v>288</v>
-      </c>
-      <c r="M74" t="s">
-        <v>289</v>
-      </c>
-      <c r="N74" t="s">
-        <v>290</v>
-      </c>
-      <c r="O74" t="s">
-        <v>291</v>
-      </c>
-      <c r="P74" t="s">
         <v>292</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>